<commit_message>
2012 download files updated with new metadatal link
</commit_message>
<xml_diff>
--- a/static/download/2012/RP1_APT_ASMA_2012.xlsx
+++ b/static/download/2012/RP1_APT_ASMA_2012.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ASMA_APT" sheetId="1" r:id="rId3"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="177">
   <si>
     <t>Data source</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Meta data</t>
   </si>
   <si>
+    <t>Metadata - Single European Sky Portal</t>
+  </si>
+  <si>
     <t>Release date</t>
   </si>
   <si>
@@ -52,7 +55,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>NSA-PRU-Support@eurocontrol.int</t>
+    <t>pru-support@eurocontrol.int</t>
   </si>
   <si>
     <t>JAN-DEC</t>
@@ -565,12 +568,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="mmm-yy"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="mmm-yy"/>
+    <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -590,8 +593,8 @@
     <font>
       <u/>
       <sz val="9.0"/>
-      <color rgb="FF396EA2"/>
-      <name val="Calibri"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -612,12 +615,6 @@
     <font>
       <sz val="9.0"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="9.0"/>
-      <color rgb="FF396EA2"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -647,7 +644,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
+    <border/>
     <border>
       <left/>
       <right/>
@@ -792,216 +790,235 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="7" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="13" fillId="4" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1010,37 +1027,40 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.57"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="19.71"/>
-    <col customWidth="1" min="4" max="4" width="13.86"/>
-    <col customWidth="1" min="5" max="5" width="9.14"/>
-    <col customWidth="1" min="6" max="7" width="11.57"/>
-    <col customWidth="1" min="8" max="8" width="11.0"/>
-    <col customWidth="1" min="9" max="9" width="22.57"/>
+    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col customWidth="1" min="3" max="3" width="17.25"/>
+    <col customWidth="1" min="4" max="4" width="12.13"/>
+    <col customWidth="1" min="5" max="5" width="8.0"/>
+    <col customWidth="1" min="6" max="7" width="10.13"/>
+    <col customWidth="1" min="8" max="8" width="9.63"/>
+    <col customWidth="1" min="9" max="9" width="19.75"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -1059,9 +1079,8 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="str">
-        <f>HYPERLINK("http://prudata.webfactional.com/wiki/index.php/Arrival_sequencing_and_metering_area_(ASMA)_additional_time","ASMA additional time")</f>
-        <v>ASMA additional time</v>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="5"/>
@@ -1069,22 +1088,22 @@
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="7">
         <v>41758.0</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="7">
         <v>41274.0</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="10"/>
@@ -1107,60 +1126,60 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I4" s="13"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="18">
         <v>106211.0</v>
@@ -1178,16 +1197,16 @@
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="18">
         <v>236625.0</v>
@@ -1205,16 +1224,16 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="18">
         <v>69184.0</v>
@@ -1232,37 +1251,37 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="23"/>
       <c r="G9" s="23"/>
       <c r="H9" s="22"/>
       <c r="I9" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="18">
         <v>105476.0</v>
@@ -1280,16 +1299,16 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" s="18">
         <v>192511.0</v>
@@ -1307,37 +1326,37 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
       <c r="H12" s="22"/>
       <c r="I12" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="18">
         <v>79766.0</v>
@@ -1355,16 +1374,16 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" s="18">
         <v>42477.0</v>
@@ -1382,16 +1401,16 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E15" s="18">
         <v>81979.0</v>
@@ -1409,16 +1428,16 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E16" s="18">
         <v>119146.0</v>
@@ -1436,16 +1455,16 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E17" s="18">
         <v>229883.0</v>
@@ -1463,16 +1482,16 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E18" s="18">
         <v>53768.0</v>
@@ -1490,16 +1509,16 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E19" s="18">
         <v>67972.0</v>
@@ -1517,16 +1536,16 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E20" s="18">
         <v>212672.0</v>
@@ -1544,16 +1563,16 @@
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E21" s="18">
         <v>77940.0</v>
@@ -1571,16 +1590,16 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E22" s="18">
         <v>115297.0</v>
@@ -1598,58 +1617,58 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="23"/>
       <c r="G23" s="23"/>
       <c r="H23" s="22"/>
       <c r="I23" s="24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="23"/>
       <c r="G24" s="23"/>
       <c r="H24" s="22"/>
       <c r="I24" s="24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E25" s="18">
         <v>101862.0</v>
@@ -1667,16 +1686,16 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E26" s="18">
         <v>37472.0</v>
@@ -1694,16 +1713,16 @@
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E27" s="18">
         <v>138033.0</v>
@@ -1721,16 +1740,16 @@
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E28" s="18">
         <v>180051.0</v>
@@ -1748,16 +1767,16 @@
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E29" s="18">
         <v>46537.0</v>
@@ -1775,16 +1794,16 @@
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E30" s="18">
         <v>76348.0</v>
@@ -1802,16 +1821,16 @@
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E31" s="18">
         <v>57394.0</v>
@@ -1829,37 +1848,37 @@
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
       <c r="H32" s="22"/>
       <c r="I32" s="24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E33" s="18">
         <v>210917.0</v>
@@ -1877,37 +1896,37 @@
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
       <c r="H34" s="22"/>
       <c r="I34" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E35" s="18">
         <v>68849.0</v>
@@ -1925,16 +1944,16 @@
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E36" s="18">
         <v>42729.0</v>
@@ -1952,16 +1971,16 @@
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E37" s="18">
         <v>82359.0</v>
@@ -1979,16 +1998,16 @@
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E38" s="18">
         <v>44420.0</v>
@@ -2006,16 +2025,16 @@
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E39" s="18">
         <v>154429.0</v>
@@ -2033,16 +2052,16 @@
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E40" s="18">
         <v>61166.0</v>
@@ -2060,16 +2079,16 @@
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E41" s="18">
         <v>127816.0</v>
@@ -2087,37 +2106,37 @@
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="23"/>
       <c r="G42" s="23"/>
       <c r="H42" s="22"/>
       <c r="I42" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E43" s="18">
         <v>86706.0</v>
@@ -2135,16 +2154,16 @@
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E44" s="18">
         <v>122265.0</v>
@@ -2170,18 +2189,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.86"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="10.43"/>
-    <col customWidth="1" min="4" max="4" width="21.86"/>
-    <col customWidth="1" min="5" max="5" width="9.0"/>
-    <col customWidth="1" min="6" max="6" width="30.43"/>
+    <col customWidth="1" min="1" max="1" width="12.13"/>
+    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col customWidth="1" min="3" max="3" width="9.13"/>
+    <col customWidth="1" min="4" max="4" width="19.13"/>
+    <col customWidth="1" min="5" max="5" width="7.88"/>
+    <col customWidth="1" min="6" max="6" width="26.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2200,233 +2222,233 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="str">
-        <f>HYPERLINK("http://prudata.webfactional.com/wiki/index.php/Arrival_sequencing_and_metering_area_(ASMA)_additional_time","ASMA additional time")</f>
-        <v>ASMA additional time</v>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="7">
         <v>41274.0</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="28" t="str">
-        <f>HYPERLINK("mailto:NSA-PRU-Support@eurocontrol.int","NSA-PRU-Support@eurocontrol.int")</f>
-        <v>NSA-PRU-Support@eurocontrol.int</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="29"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+        <v>9</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="32" t="s">
         <v>144</v>
       </c>
+      <c r="C4" s="31" t="s">
+        <v>145</v>
+      </c>
       <c r="D4" s="16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="F4" s="33"/>
+        <v>147</v>
+      </c>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36" t="s">
+      <c r="A5" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="37">
+      <c r="B5" s="34"/>
+      <c r="C5" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="36">
         <v>0.0</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="37">
         <v>0.0</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="32"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C6" s="40" t="s">
+      <c r="A6" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="D6" s="41">
+      <c r="C6" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="40">
         <v>2.12515823630473</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="33"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="40" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="33"/>
+      <c r="A7" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="42"/>
+      <c r="C7" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="43"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="33"/>
+      <c r="A8" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="46"/>
+      <c r="C8" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="48"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="32"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="39"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="39"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="39"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F1"/>
-    <hyperlink r:id="rId2" ref="F2"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.86"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="10.43"/>
-    <col customWidth="1" min="4" max="4" width="21.86"/>
-    <col customWidth="1" min="5" max="5" width="12.71"/>
-    <col customWidth="1" min="6" max="6" width="28.57"/>
-    <col customWidth="1" min="7" max="7" width="8.0"/>
+    <col customWidth="1" min="1" max="1" width="11.25"/>
+    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col customWidth="1" min="3" max="3" width="9.13"/>
+    <col customWidth="1" min="4" max="4" width="19.13"/>
+    <col customWidth="1" min="5" max="5" width="11.13"/>
+    <col customWidth="1" min="6" max="6" width="25.0"/>
+    <col customWidth="1" min="7" max="7" width="7.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2445,707 +2467,707 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="str">
-        <f>HYPERLINK("http://prudata.webfactional.com/wiki/index.php/Arrival_sequencing_and_metering_area_(ASMA)_additional_time","ASMA additional time")</f>
-        <v>ASMA additional time</v>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="G1" s="5"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="7">
         <v>41316.0</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="7">
         <v>41274.0</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="28" t="str">
-        <f>HYPERLINK("mailto:NSA-PRU-Support@eurocontrol.int","NSA-PRU-Support@eurocontrol.int")</f>
-        <v>NSA-PRU-Support@eurocontrol.int</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="G2" s="10"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="51"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>153</v>
+        <v>144</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>154</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" s="52" t="s">
         <v>155</v>
       </c>
+      <c r="E5" s="51" t="s">
+        <v>156</v>
+      </c>
       <c r="F5" s="16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="53">
+      <c r="A6" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="52">
         <v>2011.0</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="53">
         <v>40544.0</v>
       </c>
-      <c r="E6" s="55" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" s="37">
+      <c r="E6" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="36">
         <v>0.0</v>
       </c>
-      <c r="G6" s="56">
+      <c r="G6" s="55">
         <v>0.0</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="57">
+      <c r="A7" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="42"/>
+      <c r="C7" s="56">
         <v>2011.0</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="57">
         <v>40575.0</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="58" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="59"/>
+      <c r="G7" s="60"/>
+    </row>
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="42"/>
+      <c r="C8" s="56">
+        <v>2011.0</v>
+      </c>
+      <c r="D8" s="57">
+        <v>40603.0</v>
+      </c>
+      <c r="E8" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="59"/>
+      <c r="G8" s="60"/>
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="56">
+        <v>2011.0</v>
+      </c>
+      <c r="D9" s="57">
+        <v>40634.0</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
+    </row>
+    <row r="10" ht="12.75" customHeight="1">
+      <c r="A10" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="42"/>
+      <c r="C10" s="56">
+        <v>2011.0</v>
+      </c>
+      <c r="D10" s="57">
+        <v>40664.0</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
+    </row>
+    <row r="11" ht="12.75" customHeight="1">
+      <c r="A11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="56">
+        <v>2011.0</v>
+      </c>
+      <c r="D11" s="57">
+        <v>40695.0</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>163</v>
+      </c>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
+    </row>
+    <row r="12" ht="12.75" customHeight="1">
+      <c r="A12" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="42"/>
+      <c r="C12" s="56">
+        <v>2011.0</v>
+      </c>
+      <c r="D12" s="57">
+        <v>40725.0</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
+    </row>
+    <row r="13" ht="12.75" customHeight="1">
+      <c r="A13" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="42"/>
+      <c r="C13" s="56">
+        <v>2011.0</v>
+      </c>
+      <c r="D13" s="57">
+        <v>40756.0</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
+    </row>
+    <row r="14" ht="12.75" customHeight="1">
+      <c r="A14" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="56">
+        <v>2011.0</v>
+      </c>
+      <c r="D14" s="57">
+        <v>40787.0</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
+    </row>
+    <row r="15" ht="12.75" customHeight="1">
+      <c r="A15" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="42"/>
+      <c r="C15" s="56">
+        <v>2011.0</v>
+      </c>
+      <c r="D15" s="57">
+        <v>40817.0</v>
+      </c>
+      <c r="E15" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
+    </row>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="42"/>
+      <c r="C16" s="56">
+        <v>2011.0</v>
+      </c>
+      <c r="D16" s="57">
+        <v>40848.0</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="46"/>
+      <c r="C17" s="61">
+        <v>2011.0</v>
+      </c>
+      <c r="D17" s="62">
+        <v>40878.0</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="F17" s="64"/>
+      <c r="G17" s="65"/>
+    </row>
+    <row r="18" ht="12.75" customHeight="1">
+      <c r="A18" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="52">
+        <v>2012.0</v>
+      </c>
+      <c r="D18" s="53">
+        <v>40909.0</v>
+      </c>
+      <c r="E18" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="61"/>
-    </row>
-    <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="57">
-        <v>2011.0</v>
-      </c>
-      <c r="D8" s="58">
-        <v>40603.0</v>
-      </c>
-      <c r="E8" s="59" t="s">
+      <c r="F18" s="36">
+        <v>2.46715442879668</v>
+      </c>
+      <c r="G18" s="66"/>
+    </row>
+    <row r="19" ht="12.75" customHeight="1">
+      <c r="A19" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" s="56">
+        <v>2012.0</v>
+      </c>
+      <c r="D19" s="57">
+        <v>40940.0</v>
+      </c>
+      <c r="E19" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="F8" s="60"/>
-      <c r="G8" s="61"/>
-    </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="57">
-        <v>2011.0</v>
-      </c>
-      <c r="D9" s="58">
-        <v>40634.0</v>
-      </c>
-      <c r="E9" s="59" t="s">
+      <c r="F19" s="40">
+        <v>2.38953363069525</v>
+      </c>
+      <c r="G19" s="60"/>
+    </row>
+    <row r="20" ht="12.75" customHeight="1">
+      <c r="A20" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="56">
+        <v>2012.0</v>
+      </c>
+      <c r="D20" s="57">
+        <v>40969.0</v>
+      </c>
+      <c r="E20" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61"/>
-    </row>
-    <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="57">
-        <v>2011.0</v>
-      </c>
-      <c r="D10" s="58">
-        <v>40664.0</v>
-      </c>
-      <c r="E10" s="59" t="s">
+      <c r="F20" s="40">
+        <v>2.23935112562892</v>
+      </c>
+      <c r="G20" s="60"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="A21" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" s="56">
+        <v>2012.0</v>
+      </c>
+      <c r="D21" s="57">
+        <v>41000.0</v>
+      </c>
+      <c r="E21" s="58" t="s">
         <v>161</v>
       </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="61"/>
-    </row>
-    <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="57">
-        <v>2011.0</v>
-      </c>
-      <c r="D11" s="58">
-        <v>40695.0</v>
-      </c>
-      <c r="E11" s="59" t="s">
+      <c r="F21" s="40">
+        <v>2.19129217001614</v>
+      </c>
+      <c r="G21" s="60"/>
+    </row>
+    <row r="22" ht="12.75" customHeight="1">
+      <c r="A22" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="56">
+        <v>2012.0</v>
+      </c>
+      <c r="D22" s="57">
+        <v>41030.0</v>
+      </c>
+      <c r="E22" s="58" t="s">
         <v>162</v>
       </c>
-      <c r="F11" s="60"/>
-      <c r="G11" s="61"/>
-    </row>
-    <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="57">
-        <v>2011.0</v>
-      </c>
-      <c r="D12" s="58">
-        <v>40725.0</v>
-      </c>
-      <c r="E12" s="59" t="s">
+      <c r="F22" s="40">
+        <v>1.95946265637569</v>
+      </c>
+      <c r="G22" s="60"/>
+    </row>
+    <row r="23" ht="12.75" customHeight="1">
+      <c r="A23" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="56">
+        <v>2012.0</v>
+      </c>
+      <c r="D23" s="57">
+        <v>41061.0</v>
+      </c>
+      <c r="E23" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="F12" s="60"/>
-      <c r="G12" s="61"/>
-    </row>
-    <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="57">
-        <v>2011.0</v>
-      </c>
-      <c r="D13" s="58">
-        <v>40756.0</v>
-      </c>
-      <c r="E13" s="59" t="s">
+      <c r="F23" s="40">
+        <v>2.10249593024193</v>
+      </c>
+      <c r="G23" s="60"/>
+    </row>
+    <row r="24" ht="12.75" customHeight="1">
+      <c r="A24" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="56">
+        <v>2012.0</v>
+      </c>
+      <c r="D24" s="57">
+        <v>41091.0</v>
+      </c>
+      <c r="E24" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="F13" s="60"/>
-      <c r="G13" s="61"/>
-    </row>
-    <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="57">
-        <v>2011.0</v>
-      </c>
-      <c r="D14" s="58">
-        <v>40787.0</v>
-      </c>
-      <c r="E14" s="59" t="s">
+      <c r="F24" s="40">
+        <v>1.82874313458504</v>
+      </c>
+      <c r="G24" s="60"/>
+    </row>
+    <row r="25" ht="12.75" customHeight="1">
+      <c r="A25" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="56">
+        <v>2012.0</v>
+      </c>
+      <c r="D25" s="57">
+        <v>41122.0</v>
+      </c>
+      <c r="E25" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="F14" s="60"/>
-      <c r="G14" s="61"/>
-    </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="57">
-        <v>2011.0</v>
-      </c>
-      <c r="D15" s="58">
-        <v>40817.0</v>
-      </c>
-      <c r="E15" s="59" t="s">
+      <c r="F25" s="40">
+        <v>1.65224056954627</v>
+      </c>
+      <c r="G25" s="60"/>
+    </row>
+    <row r="26" ht="12.75" customHeight="1">
+      <c r="A26" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="56">
+        <v>2012.0</v>
+      </c>
+      <c r="D26" s="57">
+        <v>41153.0</v>
+      </c>
+      <c r="E26" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="F15" s="60"/>
-      <c r="G15" s="61"/>
-    </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="57">
-        <v>2011.0</v>
-      </c>
-      <c r="D16" s="58">
-        <v>40848.0</v>
-      </c>
-      <c r="E16" s="59" t="s">
+      <c r="F26" s="40">
+        <v>1.99481349870619</v>
+      </c>
+      <c r="G26" s="60"/>
+    </row>
+    <row r="27" ht="12.75" customHeight="1">
+      <c r="A27" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" s="56">
+        <v>2012.0</v>
+      </c>
+      <c r="D27" s="57">
+        <v>41183.0</v>
+      </c>
+      <c r="E27" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61"/>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="62">
-        <v>2011.0</v>
-      </c>
-      <c r="D17" s="63">
-        <v>40878.0</v>
-      </c>
-      <c r="E17" s="64" t="s">
+      <c r="F27" s="40">
+        <v>2.2414690421935</v>
+      </c>
+      <c r="G27" s="60"/>
+    </row>
+    <row r="28" ht="12.75" customHeight="1">
+      <c r="A28" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B28" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="56">
+        <v>2012.0</v>
+      </c>
+      <c r="D28" s="57">
+        <v>41214.0</v>
+      </c>
+      <c r="E28" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="F17" s="65"/>
-      <c r="G17" s="66"/>
-    </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="C18" s="53">
+      <c r="F28" s="40">
+        <v>2.17347849351344</v>
+      </c>
+      <c r="G28" s="60"/>
+    </row>
+    <row r="29" ht="12.75" customHeight="1">
+      <c r="A29" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="61">
         <v>2012.0</v>
       </c>
-      <c r="D18" s="54">
-        <v>40909.0</v>
-      </c>
-      <c r="E18" s="55" t="s">
-        <v>157</v>
-      </c>
-      <c r="F18" s="37">
-        <v>2.46715442879668</v>
-      </c>
-      <c r="G18" s="67"/>
-    </row>
-    <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" s="57">
-        <v>2012.0</v>
-      </c>
-      <c r="D19" s="58">
-        <v>40940.0</v>
-      </c>
-      <c r="E19" s="59" t="s">
-        <v>158</v>
-      </c>
-      <c r="F19" s="41">
-        <v>2.38953363069525</v>
-      </c>
-      <c r="G19" s="61"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" s="57">
-        <v>2012.0</v>
-      </c>
-      <c r="D20" s="58">
-        <v>40969.0</v>
-      </c>
-      <c r="E20" s="59" t="s">
-        <v>159</v>
-      </c>
-      <c r="F20" s="41">
-        <v>2.23935112562892</v>
-      </c>
-      <c r="G20" s="61"/>
-    </row>
-    <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C21" s="57">
-        <v>2012.0</v>
-      </c>
-      <c r="D21" s="58">
-        <v>41000.0</v>
-      </c>
-      <c r="E21" s="59" t="s">
-        <v>160</v>
-      </c>
-      <c r="F21" s="41">
-        <v>2.19129217001614</v>
-      </c>
-      <c r="G21" s="61"/>
-    </row>
-    <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="57">
-        <v>2012.0</v>
-      </c>
-      <c r="D22" s="58">
-        <v>41030.0</v>
-      </c>
-      <c r="E22" s="59" t="s">
-        <v>161</v>
-      </c>
-      <c r="F22" s="41">
-        <v>1.95946265637569</v>
-      </c>
-      <c r="G22" s="61"/>
-    </row>
-    <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C23" s="57">
-        <v>2012.0</v>
-      </c>
-      <c r="D23" s="58">
-        <v>41061.0</v>
-      </c>
-      <c r="E23" s="59" t="s">
-        <v>162</v>
-      </c>
-      <c r="F23" s="41">
-        <v>2.10249593024193</v>
-      </c>
-      <c r="G23" s="61"/>
-    </row>
-    <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C24" s="57">
-        <v>2012.0</v>
-      </c>
-      <c r="D24" s="58">
-        <v>41091.0</v>
-      </c>
-      <c r="E24" s="59" t="s">
-        <v>163</v>
-      </c>
-      <c r="F24" s="41">
-        <v>1.82874313458504</v>
-      </c>
-      <c r="G24" s="61"/>
-    </row>
-    <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C25" s="57">
-        <v>2012.0</v>
-      </c>
-      <c r="D25" s="58">
-        <v>41122.0</v>
-      </c>
-      <c r="E25" s="59" t="s">
-        <v>164</v>
-      </c>
-      <c r="F25" s="41">
-        <v>1.65224056954627</v>
-      </c>
-      <c r="G25" s="61"/>
-    </row>
-    <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B26" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C26" s="57">
-        <v>2012.0</v>
-      </c>
-      <c r="D26" s="58">
-        <v>41153.0</v>
-      </c>
-      <c r="E26" s="59" t="s">
-        <v>165</v>
-      </c>
-      <c r="F26" s="41">
-        <v>1.99481349870619</v>
-      </c>
-      <c r="G26" s="61"/>
-    </row>
-    <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C27" s="57">
-        <v>2012.0</v>
-      </c>
-      <c r="D27" s="58">
-        <v>41183.0</v>
-      </c>
-      <c r="E27" s="59" t="s">
-        <v>166</v>
-      </c>
-      <c r="F27" s="41">
-        <v>2.2414690421935</v>
-      </c>
-      <c r="G27" s="61"/>
-    </row>
-    <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C28" s="57">
-        <v>2012.0</v>
-      </c>
-      <c r="D28" s="58">
-        <v>41214.0</v>
-      </c>
-      <c r="E28" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="F28" s="41">
-        <v>2.17347849351344</v>
-      </c>
-      <c r="G28" s="61"/>
-    </row>
-    <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="B29" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="C29" s="62">
-        <v>2012.0</v>
-      </c>
-      <c r="D29" s="63">
+      <c r="D29" s="62">
         <v>41244.0</v>
       </c>
-      <c r="E29" s="64" t="s">
-        <v>168</v>
-      </c>
-      <c r="F29" s="68">
+      <c r="E29" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="F29" s="67">
         <v>2.49334109139213</v>
       </c>
-      <c r="G29" s="66"/>
+      <c r="G29" s="65"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F1"/>
-    <hyperlink r:id="rId2" ref="F2"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.57"/>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="8.0"/>
-    <col customWidth="1" min="4" max="4" width="113.57"/>
-    <col customWidth="1" min="5" max="6" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="9.25"/>
+    <col customWidth="1" min="2" max="2" width="15.88"/>
+    <col customWidth="1" min="3" max="3" width="7.0"/>
+    <col customWidth="1" min="4" max="4" width="99.38"/>
+    <col customWidth="1" min="5" max="6" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>142</v>
-      </c>
-      <c r="C1" s="69" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="70" t="s">
-        <v>17</v>
+      <c r="B1" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="71">
+      <c r="A2" s="70">
         <v>41320.0</v>
       </c>
-      <c r="B2" s="72" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="73" t="s">
+      <c r="B2" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="C2" s="72" t="s">
         <v>173</v>
       </c>
+      <c r="D2" s="71" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="71">
+      <c r="A3" s="70">
         <v>41547.0</v>
       </c>
-      <c r="B3" s="72" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="74"/>
+      <c r="B3" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="73"/>
       <c r="D3" s="20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="71">
+      <c r="A4" s="70">
         <v>41758.0</v>
       </c>
-      <c r="B4" s="72" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" s="75">
+      <c r="B4" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="74">
         <v>2012.0</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="31"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="30"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="76"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="39"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="38"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="76"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="39"/>
+      <c r="A7" s="75"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="38"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="76"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="39"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="38"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="76"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="39"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="38"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="76"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="39"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="38"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="76"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="39"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="38"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="76"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="39"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="38"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="76"/>
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="39"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="38"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="76"/>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="39"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="76"/>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="39"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="38"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="76"/>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="39"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="38"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="76"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="39"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="38"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="76"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="39"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="38"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="76"/>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="39"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="38"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="76"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="39"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="38"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>